<commit_message>
bubble chamber data update
</commit_message>
<xml_diff>
--- a/Bubble-chambers/Foglio Lavoro Bolle .xlsx
+++ b/Bubble-chambers/Foglio Lavoro Bolle .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giogi/Documents/LabFNS2/Bubble-chambers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60EC1FF-A341-9C46-B7CF-EACFD744D444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146C2DB7-D0A5-9946-AA76-45D2DC008F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{02BEFC14-27FA-2546-B417-EAD54D17AC79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{02BEFC14-27FA-2546-B417-EAD54D17AC79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sez Urto" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
   <si>
     <t>N.FOTOGRAMMA</t>
   </si>
@@ -373,13 +373,40 @@
   </si>
   <si>
     <t>025-2</t>
+  </si>
+  <si>
+    <t>Total decays</t>
+  </si>
+  <si>
+    <t>3pi decays</t>
+  </si>
+  <si>
+    <t>PDG value</t>
+  </si>
+  <si>
+    <t>Errore BR</t>
+  </si>
+  <si>
+    <t>±</t>
+  </si>
+  <si>
+    <t>2 (sistematico)</t>
+  </si>
+  <si>
+    <t>1 (sistematico)</t>
+  </si>
+  <si>
+    <t>Test Z</t>
+  </si>
+  <si>
+    <t>uguale a 017-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -436,10 +463,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -480,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -490,6 +530,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -498,6 +539,8 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2605DDD4-F087-4B4A-A959-3CF55C441A72}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
@@ -1143,7 +1186,7 @@
       <c r="H27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="10">
         <v>46.5</v>
       </c>
       <c r="K27" t="s">
@@ -1205,7 +1248,7 @@
       <c r="J34" s="8">
         <v>1.6</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="11">
         <v>2.0390000000000001E-20</v>
       </c>
     </row>
@@ -1213,7 +1256,7 @@
       <c r="H35" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J35" s="14">
+      <c r="J35" s="15">
         <v>2.0129999999999999</v>
       </c>
     </row>
@@ -1229,7 +1272,7 @@
       <c r="H37" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="11">
         <v>6.0220000000000003E+23</v>
       </c>
     </row>
@@ -1369,14 +1412,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="12">
         <f>J35/(J36*J37*E27)*LN(I48/I49)</f>
         <v>2.296442691919403E-25</v>
       </c>
       <c r="I43" t="s">
         <v>54</v>
       </c>
-      <c r="J43" s="11">
+      <c r="J43" s="12">
         <f>(K34/E27)*LN(I48/I49)</f>
         <v>1.9750992620017236E-22</v>
       </c>
@@ -1401,7 +1444,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="12">
         <f>H43*1E+24</f>
         <v>0.22964426919194031</v>
       </c>
@@ -1412,7 +1455,7 @@
         <f>SQRT(POWER(I54*E28,2) + POWER(I55*SQRT(I48),2) + POWER(I56*SQRT(I49),2))</f>
         <v>4.8569578786369791E-2</v>
       </c>
-      <c r="L44" s="16">
+      <c r="L44" s="17">
         <f>K44/H44*100</f>
         <v>21.149919811747868</v>
       </c>
@@ -1653,7 +1696,7 @@
       <c r="H54" t="s">
         <v>58</v>
       </c>
-      <c r="I54" s="11">
+      <c r="I54" s="12">
         <f>H44/E27</f>
         <v>5.8242270530499763E-3</v>
       </c>
@@ -1684,7 +1727,7 @@
       <c r="H55" t="s">
         <v>60</v>
       </c>
-      <c r="I55" s="11">
+      <c r="I55" s="12">
         <f>J35/(J36*J37*E27)/I48*1E+24</f>
         <v>1.5906506104842735E-3</v>
       </c>
@@ -1715,7 +1758,7 @@
       <c r="H56" t="s">
         <v>61</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="12">
         <f>-J35/(J36*J37*E27*I49)*1E+24</f>
         <v>-2.3304881037327732E-3</v>
       </c>
@@ -1850,13 +1893,13 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="13" t="s">
         <v>80</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
-      <c r="E63" s="12"/>
+      <c r="E63" s="13"/>
       <c r="F63">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1875,7 +1918,7 @@
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="14">
         <v>6</v>
       </c>
       <c r="F64">
@@ -2232,7 +2275,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B81">
@@ -2400,7 +2443,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2408,25 +2451,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B14B55B-8003-8B4B-8DBF-93AEA3F4FB22}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="3" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2436,13 +2485,625 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="8" t="s">
+      <c r="F3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B4:B59)</f>
+        <v>621</v>
+      </c>
+      <c r="G4">
+        <f>SUM(C4:C59)</f>
+        <v>40</v>
+      </c>
+      <c r="I4" s="18">
+        <v>5.5830000000000002</v>
+      </c>
+      <c r="J4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
         <v>8</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="10">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="F14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="10">
+        <v>18</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15">
+        <f>G4/F4</f>
+        <v>6.4412238325281798E-2</v>
+      </c>
+      <c r="F15">
+        <f>SQRT(E15*(1-E15)/F4)</f>
+        <v>9.8510077694010656E-3</v>
+      </c>
+      <c r="H15">
+        <f>F15/E15*100</f>
+        <v>15.293689561995155</v>
+      </c>
+      <c r="I15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="10">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16">
+        <f>E15*100</f>
+        <v>6.4412238325281796</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="10">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="10">
+        <v>16</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="10">
+        <v>13</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f>ABS(E15*100-I4)/SQRT(K4^2+(F15*100)^2)</f>
+        <v>0.87094565784975497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="10">
+        <v>7</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="10">
+        <v>14</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="10">
+        <v>10</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="10">
+        <v>3</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="10">
+        <v>11</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="10">
+        <v>10</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="10">
+        <v>6</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="10">
+        <v>10</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="10">
+        <v>16</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="10">
+        <v>9</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="10">
+        <v>12</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="10">
+        <v>13</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="10">
+        <v>15</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="10">
+        <v>15</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="10">
+        <v>16</v>
+      </c>
+      <c r="C34" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="10">
+        <v>10</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="10">
+        <v>11</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="10">
+        <v>23</v>
+      </c>
+      <c r="C37" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42">
+        <v>17</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53">
+        <v>16</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add syst Anti P and K
</commit_message>
<xml_diff>
--- a/Bubble-chambers/Foglio Lavoro Bolle .xlsx
+++ b/Bubble-chambers/Foglio Lavoro Bolle .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\LabFNS2\Bubble-chambers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A79E6A-A827-4CBA-9A3D-38FBEA056BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE40A373-56E6-4758-A5B1-49AC8D93784E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="173">
   <si>
     <t>MISURA DELLA SEZIONE D'URTO ANTIPROTONI-DEUTERIO P_lab=1,6 GeV/c</t>
   </si>
@@ -547,6 +547,18 @@
   </si>
   <si>
     <t>047-2</t>
+  </si>
+  <si>
+    <t>ANTI P</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>3P</t>
+  </si>
+  <si>
+    <t>Tot dec</t>
   </si>
 </sst>
 </file>
@@ -638,7 +650,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,6 +673,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -758,9 +776,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -789,7 +804,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1317,47 +1335,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2"/>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1390,66 +1408,66 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:11" s="2" customFormat="1">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>-5.1700000000000003E-2</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>8.5736000000000008</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>-8.7030999999999992</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>-7.4099999999999999E-2</v>
       </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
         <v>-2.9499999999999998E-2</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>-4.99E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:11" s="2" customFormat="1">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>29.970300000000002</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>14.975199999999999</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>14.985900000000001</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>-5.5999999999999999E-3</v>
       </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
         <v>23.232700000000001</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>-4.9466000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1482,76 +1500,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="3" customFormat="1">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:11" s="2" customFormat="1">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>8.6404999999999994</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>-8.641</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>8.6417999999999999</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>-8.6408000000000005</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>-1.6500000000000001E-2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>-1.3899999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:11" s="2" customFormat="1">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>29.970300000000002</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>14.9801</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>14.9838</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>-4.3E-3</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>-14.9252</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>-14.9831</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>23.238299999999999</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>-4.9396000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="5" customFormat="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="1:11" s="4" customFormat="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1572,7 +1590,7 @@
         <f>I31/D27</f>
         <v>39.429140914360879</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I27">
@@ -1592,7 +1610,7 @@
       <c r="F28" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I28">
@@ -1600,7 +1618,7 @@
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I29">
@@ -1609,7 +1627,7 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I30">
@@ -1618,7 +1636,7 @@
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I31">
@@ -1626,42 +1644,42 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="7" customFormat="1">
-      <c r="H34" s="7" t="s">
+    <row r="34" spans="1:13" s="6" customFormat="1">
+      <c r="H34" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="6">
         <v>1.6</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="7">
         <v>2.0390000000000001E-20</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="7" customFormat="1">
-      <c r="H35" s="7" t="s">
+    <row r="35" spans="1:13" s="6" customFormat="1">
+      <c r="H35" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="8">
         <v>2.0129999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="7" customFormat="1">
-      <c r="H36" s="7" t="s">
+    <row r="36" spans="1:13" s="6" customFormat="1">
+      <c r="H36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="7">
+      <c r="J36" s="6">
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="7" customFormat="1">
-      <c r="H37" s="7" t="s">
+    <row r="37" spans="1:13" s="6" customFormat="1">
+      <c r="H37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="8">
+      <c r="J37" s="7">
         <v>6.0220000000000003E+23</v>
       </c>
     </row>
@@ -1705,7 +1723,7 @@
         <f t="shared" ref="F39:F70" si="0">B39-(D39+C39+E39)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="H39" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1771,13 +1789,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="9" t="s">
         <v>43</v>
       </c>
       <c r="K42" t="s">
         <v>44</v>
       </c>
-      <c r="L42" s="10" t="s">
+      <c r="L42" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1801,14 +1819,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="10">
         <f>$J$35/($J$36*$J$37*$E$27)*LN(I48/I49)</f>
         <v>2.2676421778333534E-25</v>
       </c>
       <c r="I43" t="s">
         <v>47</v>
       </c>
-      <c r="J43" s="11">
+      <c r="J43" s="10">
         <f>(K34/E27)*LN(I48/I49)</f>
         <v>1.950328831493361E-22</v>
       </c>
@@ -1833,7 +1851,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="10">
         <f>H43*1E+24</f>
         <v>0.22676421778333533</v>
       </c>
@@ -1844,7 +1862,7 @@
         <f>SQRT(POWER(I54*E28,2) + POWER(I55*SQRT(I48),2) + POWER(I56*SQRT(I49),2))</f>
         <v>3.9959506104829214E-2</v>
       </c>
-      <c r="L44" s="12">
+      <c r="L44" s="11">
         <f>K44/H44*100</f>
         <v>17.621610012126787</v>
       </c>
@@ -2088,7 +2106,7 @@
       <c r="H54" t="s">
         <v>65</v>
       </c>
-      <c r="I54" s="11">
+      <c r="I54" s="10">
         <f>H44/$E$27</f>
         <v>5.7511833259532999E-3</v>
       </c>
@@ -2119,7 +2137,7 @@
       <c r="H55" t="s">
         <v>68</v>
       </c>
-      <c r="I55" s="11">
+      <c r="I55" s="10">
         <f>$J$35/($J$36*$J$37*$E$27)/I48*1E+24</f>
         <v>1.0794720480485733E-3</v>
       </c>
@@ -2150,7 +2168,7 @@
       <c r="H56" t="s">
         <v>70</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="10">
         <f>-$J$35/($J$36*$J$37*$E$27*I49)*1E+24</f>
         <v>-1.5739945831493595E-3</v>
       </c>
@@ -2241,7 +2259,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J60" s="13"/>
+      <c r="J60" s="12"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
@@ -2286,13 +2304,13 @@
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="13" t="s">
         <v>77</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
-      <c r="E63" s="14"/>
+      <c r="E63" s="13"/>
       <c r="F63">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2311,7 +2329,7 @@
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="14">
         <v>6</v>
       </c>
       <c r="F64">
@@ -2471,7 +2489,7 @@
         <v>6</v>
       </c>
       <c r="F71">
-        <f t="shared" ref="F71:F102" si="1">B71-(D71+C71+E71)</f>
+        <f t="shared" ref="F71:F88" si="1">B71-(D71+C71+E71)</f>
         <v>0</v>
       </c>
       <c r="H71" t="s">
@@ -2668,7 +2686,7 @@
       </c>
     </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B81">
@@ -2842,43 +2860,43 @@
       <c r="D92" t="s">
         <v>108</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="G92" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="H92" s="1"/>
+      <c r="H92" s="29"/>
     </row>
     <row r="93" spans="1:13">
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
     </row>
     <row r="94" spans="1:13">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B94" s="18">
+      <c r="B94" s="17">
         <v>11</v>
       </c>
-      <c r="C94" s="18">
-        <v>2</v>
-      </c>
-      <c r="D94" s="18">
+      <c r="C94" s="17">
+        <v>2</v>
+      </c>
+      <c r="D94" s="17">
         <v>3</v>
       </c>
-      <c r="E94" s="18">
+      <c r="E94" s="17">
         <f t="shared" ref="E94:E110" si="2">B94-C94-D94</f>
         <v>6</v>
       </c>
-      <c r="F94" s="18"/>
-      <c r="G94" s="18"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-      <c r="J94" s="18"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="18"/>
-      <c r="M94" s="19"/>
+      <c r="F94" s="17"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+      <c r="J94" s="17"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="17"/>
+      <c r="M94" s="18"/>
     </row>
     <row r="95" spans="1:13">
-      <c r="A95" s="20" t="s">
+      <c r="A95" s="19" t="s">
         <v>111</v>
       </c>
       <c r="B95">
@@ -2894,19 +2912,19 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H95" s="10" t="s">
+      <c r="H95" s="9" t="s">
         <v>43</v>
       </c>
       <c r="K95" t="s">
         <v>44</v>
       </c>
-      <c r="L95" s="10" t="s">
+      <c r="L95" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="M95" s="21"/>
+      <c r="M95" s="20"/>
     </row>
     <row r="96" spans="1:13">
-      <c r="A96" s="20" t="s">
+      <c r="A96" s="19" t="s">
         <v>112</v>
       </c>
       <c r="B96">
@@ -2922,21 +2940,21 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H96" s="11">
+      <c r="H96" s="10">
         <f>$J$35/($J$36*$J$37*$E$27)*LN(I101/I102)</f>
         <v>2.3351405523395175E-25</v>
       </c>
       <c r="I96" t="s">
         <v>47</v>
       </c>
-      <c r="J96" s="11">
+      <c r="J96" s="10">
         <f>(K87/E80)*LN(I101/I102)</f>
         <v>0</v>
       </c>
-      <c r="M96" s="21"/>
+      <c r="M96" s="20"/>
     </row>
     <row r="97" spans="1:13">
-      <c r="A97" s="20" t="s">
+      <c r="A97" s="19" t="s">
         <v>113</v>
       </c>
       <c r="B97">
@@ -2952,7 +2970,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H97" s="11">
+      <c r="H97" s="10">
         <f>H96*1E+24</f>
         <v>0.23351405523395175</v>
       </c>
@@ -2963,16 +2981,16 @@
         <f>SQRT(POWER(I107*E81,2) + POWER(I108*SQRT(I101),2) + POWER(I109*SQRT(I102),2))</f>
         <v>0.10563968362764495</v>
       </c>
-      <c r="L97" s="12">
+      <c r="L97" s="11">
         <f>K97/H97*100</f>
         <v>45.239111419570548</v>
       </c>
-      <c r="M97" s="21" t="s">
+      <c r="M97" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:13">
-      <c r="A98" s="20" t="s">
+      <c r="A98" s="19" t="s">
         <v>114</v>
       </c>
       <c r="B98">
@@ -2988,10 +3006,10 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="M98" s="21"/>
+      <c r="M98" s="20"/>
     </row>
     <row r="99" spans="1:13">
-      <c r="A99" s="20" t="s">
+      <c r="A99" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B99">
@@ -3007,10 +3025,10 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="M99" s="21"/>
+      <c r="M99" s="20"/>
     </row>
     <row r="100" spans="1:13">
-      <c r="A100" s="20" t="s">
+      <c r="A100" s="19" t="s">
         <v>116</v>
       </c>
       <c r="B100">
@@ -3026,10 +3044,10 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="M100" s="21"/>
+      <c r="M100" s="20"/>
     </row>
     <row r="101" spans="1:13">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="19" t="s">
         <v>117</v>
       </c>
       <c r="B101">
@@ -3056,10 +3074,10 @@
         <f>I107*E81</f>
         <v>2.961186191466085E-2</v>
       </c>
-      <c r="M101" s="21"/>
+      <c r="M101" s="20"/>
     </row>
     <row r="102" spans="1:13">
-      <c r="A102" s="20" t="s">
+      <c r="A102" s="19" t="s">
         <v>118</v>
       </c>
       <c r="B102">
@@ -3082,10 +3100,10 @@
         <f>SUM(E94:E110)</f>
         <v>59</v>
       </c>
-      <c r="M102" s="21"/>
+      <c r="M102" s="20"/>
     </row>
     <row r="103" spans="1:13">
-      <c r="A103" s="20" t="s">
+      <c r="A103" s="19" t="s">
         <v>119</v>
       </c>
       <c r="B103">
@@ -3101,10 +3119,10 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="M103" s="21"/>
+      <c r="M103" s="20"/>
     </row>
     <row r="104" spans="1:13">
-      <c r="A104" s="20" t="s">
+      <c r="A104" s="19" t="s">
         <v>120</v>
       </c>
       <c r="B104">
@@ -3120,10 +3138,10 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="M104" s="21"/>
+      <c r="M104" s="20"/>
     </row>
     <row r="105" spans="1:13">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="19" t="s">
         <v>121</v>
       </c>
       <c r="B105">
@@ -3139,10 +3157,10 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="M105" s="21"/>
+      <c r="M105" s="20"/>
     </row>
     <row r="106" spans="1:13">
-      <c r="A106" s="20"/>
+      <c r="A106" s="19"/>
       <c r="E106">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3150,10 +3168,10 @@
       <c r="H106" t="s">
         <v>63</v>
       </c>
-      <c r="M106" s="21"/>
+      <c r="M106" s="20"/>
     </row>
     <row r="107" spans="1:13">
-      <c r="A107" s="20"/>
+      <c r="A107" s="19"/>
       <c r="E107">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3161,17 +3179,17 @@
       <c r="H107" t="s">
         <v>65</v>
       </c>
-      <c r="I107" s="11">
+      <c r="I107" s="10">
         <f>H97/$E$27</f>
         <v>5.9223723829321699E-3</v>
       </c>
       <c r="J107" t="s">
         <v>66</v>
       </c>
-      <c r="M107" s="21"/>
+      <c r="M107" s="20"/>
     </row>
     <row r="108" spans="1:13">
-      <c r="A108" s="20"/>
+      <c r="A108" s="19"/>
       <c r="E108">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3179,17 +3197,17 @@
       <c r="H108" t="s">
         <v>68</v>
       </c>
-      <c r="I108" s="11">
+      <c r="I108" s="10">
         <f>$J$35/($J$36*$J$37*$E$27)/I101*1E+24</f>
         <v>6.9111026524489132E-3</v>
       </c>
       <c r="J108" t="s">
         <v>49</v>
       </c>
-      <c r="M108" s="21"/>
+      <c r="M108" s="20"/>
     </row>
     <row r="109" spans="1:13">
-      <c r="A109" s="20"/>
+      <c r="A109" s="19"/>
       <c r="E109">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3197,65 +3215,65 @@
       <c r="H109" t="s">
         <v>70</v>
       </c>
-      <c r="I109" s="11">
+      <c r="I109" s="10">
         <f>-$J$35/($J$36*$J$37*$E$27*I102)*1E+24</f>
         <v>-1.0190947979034836E-2</v>
       </c>
       <c r="J109" t="s">
         <v>49</v>
       </c>
-      <c r="M109" s="21"/>
+      <c r="M109" s="20"/>
     </row>
     <row r="110" spans="1:13">
-      <c r="A110" s="22"/>
-      <c r="B110" s="23"/>
-      <c r="C110" s="23"/>
-      <c r="D110" s="23"/>
-      <c r="E110" s="23">
+      <c r="A110" s="21"/>
+      <c r="B110" s="22"/>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F110" s="23"/>
-      <c r="G110" s="23"/>
-      <c r="H110" s="23"/>
-      <c r="I110" s="23"/>
-      <c r="J110" s="23"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="23"/>
-      <c r="M110" s="24"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="22"/>
+      <c r="I110" s="22"/>
+      <c r="J110" s="22"/>
+      <c r="K110" s="22"/>
+      <c r="L110" s="22"/>
+      <c r="M110" s="23"/>
     </row>
     <row r="112" spans="1:13">
-      <c r="G112" s="1" t="s">
+      <c r="G112" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="H112" s="1"/>
+      <c r="H112" s="29"/>
     </row>
     <row r="113" spans="1:13">
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
+      <c r="G113" s="29"/>
+      <c r="H113" s="29"/>
     </row>
     <row r="114" spans="1:13">
-      <c r="A114" s="18" t="s">
+      <c r="A114" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C114" s="18" t="s">
+      <c r="C114" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="D114" s="18" t="s">
+      <c r="D114" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="18"/>
-      <c r="L114" s="18"/>
-      <c r="M114" s="18"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
+      <c r="J114" s="17"/>
+      <c r="K114" s="17"/>
+      <c r="L114" s="17"/>
+      <c r="M114" s="17"/>
     </row>
     <row r="115" spans="1:13">
       <c r="A115" t="s">
@@ -3292,7 +3310,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="H116" s="10" t="s">
+      <c r="H116" s="9" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3459,25 +3477,25 @@
       </c>
     </row>
     <row r="126" spans="1:13">
-      <c r="A126" s="23" t="s">
+      <c r="A126" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="B126" s="23">
+      <c r="B126" s="22">
         <v>9</v>
       </c>
-      <c r="C126" s="23">
-        <v>0</v>
-      </c>
-      <c r="D126" s="23">
-        <v>1</v>
-      </c>
-      <c r="E126" s="25">
+      <c r="C126" s="22">
+        <v>0</v>
+      </c>
+      <c r="D126" s="22">
+        <v>1</v>
+      </c>
+      <c r="E126" s="24">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="F126" s="23"/>
-      <c r="G126" s="23"/>
-      <c r="H126" s="23"/>
+      <c r="F126" s="22"/>
+      <c r="G126" s="22"/>
+      <c r="H126" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3492,10 +3510,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
@@ -3511,8 +3529,8 @@
     <col min="12" max="12" width="2.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="26" customFormat="1">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:12" s="25" customFormat="1">
+      <c r="A1" s="25" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3532,7 +3550,7 @@
       <c r="G3" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3554,7 +3572,7 @@
         <f>SUM(C4:C59)</f>
         <v>40</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="27">
         <v>5.5830000000000002</v>
       </c>
       <c r="J4" t="s">
@@ -3666,28 +3684,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="7" customFormat="1">
-      <c r="A14" s="29" t="s">
+    <row r="14" spans="1:12" s="6" customFormat="1">
+      <c r="A14" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>59</v>
       </c>
       <c r="B15">
@@ -3716,7 +3734,7 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>60</v>
       </c>
       <c r="B16">
@@ -3737,7 +3755,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B17">
@@ -3748,7 +3766,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>62</v>
       </c>
       <c r="B18">
@@ -3757,12 +3775,12 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>64</v>
       </c>
       <c r="B19">
@@ -3777,7 +3795,7 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>67</v>
       </c>
       <c r="B20">
@@ -3788,7 +3806,7 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>69</v>
       </c>
       <c r="B21">
@@ -3799,7 +3817,7 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>71</v>
       </c>
       <c r="B22">
@@ -3810,7 +3828,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>72</v>
       </c>
       <c r="B23">
@@ -3821,7 +3839,7 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="28" t="s">
         <v>73</v>
       </c>
       <c r="B24">
@@ -3832,7 +3850,7 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="28" t="s">
         <v>74</v>
       </c>
       <c r="B25">
@@ -3843,7 +3861,7 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B26">
@@ -3854,7 +3872,7 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B27">
@@ -3865,7 +3883,7 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B28">
@@ -3876,7 +3894,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B29">
@@ -3887,7 +3905,7 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B30">
@@ -3898,7 +3916,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>81</v>
       </c>
       <c r="B31">
@@ -3909,7 +3927,7 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B32">
@@ -3920,7 +3938,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>84</v>
       </c>
       <c r="B33">
@@ -3931,7 +3949,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B34">
@@ -3942,7 +3960,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B35">
@@ -3953,7 +3971,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="28" t="s">
         <v>88</v>
       </c>
       <c r="B36">
@@ -3964,7 +3982,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B37">
@@ -3975,7 +3993,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>91</v>
       </c>
       <c r="D38" t="s">
@@ -3983,7 +4001,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>92</v>
       </c>
       <c r="B39">
@@ -3994,7 +4012,7 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>93</v>
       </c>
       <c r="B40">
@@ -4005,7 +4023,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>94</v>
       </c>
       <c r="B41">
@@ -4016,7 +4034,7 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="28" t="s">
         <v>95</v>
       </c>
       <c r="B42">
@@ -4027,7 +4045,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="28" t="s">
         <v>96</v>
       </c>
       <c r="B43">
@@ -4038,7 +4056,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="28" t="s">
         <v>97</v>
       </c>
       <c r="B44">
@@ -4049,7 +4067,7 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="28" t="s">
         <v>98</v>
       </c>
       <c r="B45">
@@ -4060,7 +4078,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B46">
@@ -4071,7 +4089,7 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B47">
@@ -4082,7 +4100,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="28" t="s">
         <v>101</v>
       </c>
       <c r="B48">
@@ -4093,7 +4111,7 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B49">
@@ -4104,7 +4122,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="28" t="s">
         <v>103</v>
       </c>
       <c r="B50">
@@ -4115,7 +4133,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B51">
@@ -4126,7 +4144,7 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B52">
@@ -4137,7 +4155,7 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>106</v>
       </c>
       <c r="B53">
@@ -4146,6 +4164,18 @@
       <c r="C53">
         <v>3</v>
       </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="28"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="28"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="28"/>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4441,10 +4471,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15.6"/>
@@ -4453,15 +4483,24 @@
     <col min="4" max="4" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="C1" t="s">
         <v>107</v>
       </c>
       <c r="D1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -4479,7 +4518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -4497,7 +4536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>157</v>
       </c>
@@ -4515,7 +4554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -4533,7 +4572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -4551,7 +4590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -4569,7 +4608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -4587,7 +4626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -4604,59 +4643,239 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>162</v>
       </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>163</v>
       </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>164</v>
       </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>165</v>
       </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>166</v>
       </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>167</v>
       </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
       <c r="E15">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
directory rearranged. Fixed problemmss in preprocessor
</commit_message>
<xml_diff>
--- a/Bubble-chambers/Foglio Lavoro Bolle .xlsx
+++ b/Bubble-chambers/Foglio Lavoro Bolle .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giogi/Documents/LabFNS2/Bubble-chambers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA8D426-724F-E142-BD16-6B6AB0DEA5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5754D7-E09E-7A45-8285-1F91CDC57AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sez Urto" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="176">
   <si>
     <t>MISURA DELLA SEZIONE D'URTO ANTIPROTONI-DEUTERIO P_lab=1,6 GeV/c</t>
   </si>
@@ -565,6 +565,9 @@
   </si>
   <si>
     <t>047-2</t>
+  </si>
+  <si>
+    <t>Anti-p entranti</t>
   </si>
 </sst>
 </file>
@@ -1240,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView topLeftCell="C103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3418,7 +3421,6 @@
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="23"/>
-      <c r="H126" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3435,7 +3437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4110,7 +4112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -4938,17 +4940,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:K17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>175</v>
+      </c>
       <c r="C1" t="s">
         <v>107</v>
       </c>
@@ -4969,126 +4975,252 @@
       <c r="A2" t="s">
         <v>155</v>
       </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
       <c r="E2">
         <f t="shared" ref="E2:E15" si="0">B2-C2-D2</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>156</v>
       </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>157</v>
       </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>158</v>
       </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>159</v>
       </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>160</v>
       </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>161</v>
       </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>161</v>
       </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>162</v>
       </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>163</v>
       </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>164</v>
       </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>165</v>
       </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>166</v>
       </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>167</v>
       </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -5124,7 +5256,7 @@
         <v>111</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -5135,7 +5267,7 @@
         <v>112</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -5146,10 +5278,10 @@
         <v>113</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -5160,7 +5292,7 @@
         <v>14</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -5168,10 +5300,10 @@
         <v>115</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -5182,7 +5314,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -5190,7 +5322,7 @@
         <v>117</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -5201,10 +5333,10 @@
         <v>118</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -5212,7 +5344,7 @@
         <v>119</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>0</v>

</xml_diff>